<commit_message>
EPBDS-9810 fix casting issues
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-8949_DifferentTypesInSpreadsheets.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-8949_DifferentTypesInSpreadsheets.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CCF56AE-0776-4A64-80F7-65DE55F0B9B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{441829D6-F369-48DC-ABA0-57D22E64B8A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15945" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="11" r:id="rId1"/>
@@ -304,9 +304,6 @@
     <t>= instanceOf($Value, Long.class)</t>
   </si>
   <si>
-    <t>_res_.$Value$B[0]</t>
-  </si>
-  <si>
     <t>_res_.$Value$C</t>
   </si>
   <si>
@@ -479,6 +476,9 @@
   </si>
   <si>
     <t>Spreadsheet SpreadsheetResult Inner2()</t>
+  </si>
+  <si>
+    <t>_res_.$Value$B</t>
   </si>
 </sst>
 </file>
@@ -878,16 +878,16 @@
   <dimension ref="A1:X67"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="50.59765625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="41.3984375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="50.5546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="41.44140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -895,7 +895,7 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -903,19 +903,19 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="7" t="s">
         <v>6</v>
@@ -924,7 +924,7 @@
       <c r="D6" s="7"/>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
         <v>2</v>
@@ -937,7 +937,7 @@
       </c>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
         <v>0</v>
@@ -950,7 +950,7 @@
       </c>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
         <v>8</v>
@@ -959,11 +959,11 @@
         <v>34</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
         <v>9</v>
@@ -972,11 +972,11 @@
         <v>18</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
         <v>10</v>
@@ -985,11 +985,11 @@
         <v>29</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
         <v>19</v>
@@ -1002,7 +1002,7 @@
       </c>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
         <v>20</v>
@@ -1011,11 +1011,11 @@
         <v>24</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1" t="s">
         <v>21</v>
@@ -1028,7 +1028,7 @@
       </c>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="1" t="s">
         <v>22</v>
@@ -1037,11 +1037,11 @@
         <v>26</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="1" t="s">
         <v>23</v>
@@ -1050,11 +1050,11 @@
         <v>27</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="1" t="s">
         <v>31</v>
@@ -1063,11 +1063,11 @@
         <v>24</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="1" t="s">
         <v>32</v>
@@ -1076,11 +1076,11 @@
         <v>27</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="1" t="s">
         <v>33</v>
@@ -1089,43 +1089,43 @@
         <v>28</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="2"/>
       <c r="E21" s="1"/>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="7" t="s">
         <v>12</v>
@@ -1134,79 +1134,79 @@
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="E25" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="F25" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="G25" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G25" s="1" t="s">
+      <c r="H25" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="H25" s="1" t="s">
+      <c r="I25" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I25" s="1" t="s">
+      <c r="J25" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="J25" s="1" t="s">
+      <c r="K25" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="K25" s="1" t="s">
+      <c r="L25" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="L25" s="1" t="s">
+      <c r="M25" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="N25" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="M25" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="N25" s="1" t="s">
+      <c r="O25" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="O25" s="1" t="s">
+      <c r="P25" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="P25" s="1" t="s">
+      <c r="Q25" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="Q25" s="1" t="s">
+      <c r="R25" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="R25" s="1" t="s">
+      <c r="S25" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="S25" s="1" t="s">
+      <c r="T25" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="T25" s="1" t="s">
+      <c r="U25" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="U25" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="V25" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="W25" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="W25" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="X25" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.45">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="1" t="s">
         <v>14</v>
@@ -1278,7 +1278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
       <c r="B27" s="1" t="s">
         <v>4</v>
       </c>
@@ -1313,43 +1313,43 @@
         <v>1</v>
       </c>
       <c r="M27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O27" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P27" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Q27" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="R27" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="S27" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="T27" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="U27" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="V27" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="W27" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="X27" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.45">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
       <c r="B28" s="1" t="s">
         <v>16</v>
       </c>
@@ -1384,43 +1384,43 @@
         <v>1</v>
       </c>
       <c r="M28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N28" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O28" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P28" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Q28" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="R28" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="S28" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="T28" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="U28" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="V28" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="W28" s="1" t="s">
         <v>34</v>
       </c>
       <c r="X28" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.45">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B34" s="7" t="s">
         <v>6</v>
       </c>
@@ -1431,7 +1431,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B35" s="1" t="s">
         <v>2</v>
       </c>
@@ -1442,7 +1442,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B36" s="1" t="s">
         <v>0</v>
       </c>
@@ -1453,7 +1453,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="37" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B37" s="1" t="s">
         <v>8</v>
       </c>
@@ -1461,10 +1461,10 @@
         <v>11</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.45">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B38" s="1" t="s">
         <v>9</v>
       </c>
@@ -1472,12 +1472,12 @@
         <v>17</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="39" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B39" s="1" t="s">
         <v>10</v>
       </c>
@@ -1490,7 +1490,7 @@
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="40" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B40" s="1" t="s">
         <v>19</v>
       </c>
@@ -1498,12 +1498,12 @@
         <v>24</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
     </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="41" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B41" s="1" t="s">
         <v>20</v>
       </c>
@@ -1516,7 +1516,7 @@
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
     </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="42" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B42" s="1" t="s">
         <v>21</v>
       </c>
@@ -1524,12 +1524,12 @@
         <v>26</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
     </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="43" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B43" s="1" t="s">
         <v>22</v>
       </c>
@@ -1537,12 +1537,12 @@
         <v>27</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
     </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="44" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
         <v>23</v>
       </c>
@@ -1550,12 +1550,12 @@
         <v>28</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
     </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="45" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
         <v>31</v>
       </c>
@@ -1563,12 +1563,12 @@
         <v>37</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
     </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="46" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
         <v>32</v>
       </c>
@@ -1576,12 +1576,12 @@
         <v>35</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
     </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="47" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
         <v>33</v>
       </c>
@@ -1589,41 +1589,41 @@
         <v>36</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
     </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="48" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C48" s="1"/>
       <c r="D48" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
     </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="49" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
     </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="50" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
     </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="51" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
     </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="53" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B53" s="7" t="s">
         <v>5</v>
       </c>
@@ -1631,7 +1631,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="54" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B54" s="1" t="s">
         <v>0</v>
       </c>
@@ -1642,7 +1642,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="55" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B55" s="1" t="s">
         <v>8</v>
       </c>
@@ -1650,137 +1650,137 @@
         <v>7</v>
       </c>
       <c r="D55" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.45">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="56" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B56" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.45">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B57" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="58" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B58" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.45">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B59" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="60" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B60" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.45">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="61" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B61" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="62" spans="2:6" x14ac:dyDescent="0.45">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="62" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B62" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="63" spans="2:6" x14ac:dyDescent="0.45">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="63" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B63" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="64" spans="2:6" x14ac:dyDescent="0.45">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="64" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B64" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="65" spans="2:4" x14ac:dyDescent="0.45">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B65" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C65" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B66" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C66" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D65" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B66" s="1" t="s">
+      <c r="D66" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C66" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="D66" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="67" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B67" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C67" s="2"/>
       <c r="D67" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1803,12 +1803,12 @@
       <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="21.86328125" customWidth="1"/>
+    <col min="2" max="2" width="21.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -1834,7 +1834,7 @@
       <c r="W1" s="4"/>
       <c r="X1" s="4"/>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -1860,7 +1860,7 @@
       <c r="W2" s="4"/>
       <c r="X2" s="4"/>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -1886,7 +1886,7 @@
       <c r="W3" s="4"/>
       <c r="X3" s="4"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -1912,10 +1912,10 @@
       <c r="W4" s="4"/>
       <c r="X4" s="4"/>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
       <c r="B5" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="4"/>
@@ -1940,13 +1940,13 @@
       <c r="W5" s="4"/>
       <c r="X5" s="4"/>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" s="4" t="s">
         <v>15</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
@@ -1970,7 +1970,7 @@
       <c r="W6" s="4"/>
       <c r="X6" s="4"/>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="4" t="s">
         <v>14</v>
@@ -2000,7 +2000,7 @@
       <c r="W7" s="4"/>
       <c r="X7" s="4"/>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
       <c r="B8" s="4" t="s">
         <v>4</v>
@@ -2030,7 +2030,7 @@
       <c r="W8" s="4"/>
       <c r="X8" s="4"/>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="4" t="s">
         <v>16</v>
@@ -2060,7 +2060,7 @@
       <c r="W9" s="4"/>
       <c r="X9" s="4"/>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -2086,7 +2086,7 @@
       <c r="W10" s="3"/>
       <c r="X10" s="3"/>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -2112,7 +2112,7 @@
       <c r="W11" s="3"/>
       <c r="X11" s="3"/>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -2138,7 +2138,7 @@
       <c r="W12" s="3"/>
       <c r="X12" s="3"/>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -2164,7 +2164,7 @@
       <c r="W13" s="3"/>
       <c r="X13" s="3"/>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -2190,7 +2190,7 @@
       <c r="W14" s="3"/>
       <c r="X14" s="3"/>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -2216,10 +2216,10 @@
       <c r="W15" s="3"/>
       <c r="X15" s="3"/>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="9"/>
@@ -2244,7 +2244,7 @@
       <c r="W16" s="4"/>
       <c r="X16" s="4"/>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="6" t="s">
         <v>2</v>
@@ -2276,7 +2276,7 @@
       <c r="W17" s="3"/>
       <c r="X17" s="3"/>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="4" t="s">
         <v>0</v>
@@ -2306,10 +2306,10 @@
       <c r="W18" s="3"/>
       <c r="X18" s="3"/>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
       <c r="B19" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C19" s="10" t="s">
         <v>27</v>
@@ -2336,7 +2336,7 @@
       <c r="W19" s="3"/>
       <c r="X19" s="3"/>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -2362,7 +2362,7 @@
       <c r="W20" s="3"/>
       <c r="X20" s="3"/>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -2388,7 +2388,7 @@
       <c r="W21" s="3"/>
       <c r="X21" s="3"/>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -2414,10 +2414,10 @@
       <c r="W22" s="3"/>
       <c r="X22" s="3"/>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
       <c r="B23" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>5</v>
@@ -2444,7 +2444,7 @@
       <c r="W23" s="3"/>
       <c r="X23" s="3"/>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
       <c r="B24" s="4" t="s">
         <v>0</v>
@@ -2474,13 +2474,13 @@
       <c r="W24" s="3"/>
       <c r="X24" s="3"/>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
       <c r="B25" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
@@ -2504,13 +2504,13 @@
       <c r="W25" s="3"/>
       <c r="X25" s="3"/>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A26" s="3"/>
       <c r="B26" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
@@ -2534,7 +2534,7 @@
       <c r="W26" s="3"/>
       <c r="X26" s="3"/>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -2560,7 +2560,7 @@
       <c r="W27" s="3"/>
       <c r="X27" s="3"/>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -2586,7 +2586,7 @@
       <c r="W28" s="3"/>
       <c r="X28" s="3"/>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -2612,7 +2612,7 @@
       <c r="W29" s="3"/>
       <c r="X29" s="3"/>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -2638,10 +2638,10 @@
       <c r="W30" s="3"/>
       <c r="X30" s="3"/>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A31" s="3"/>
       <c r="B31" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
@@ -2666,7 +2666,7 @@
       <c r="W31" s="3"/>
       <c r="X31" s="3"/>
     </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A32" s="3"/>
       <c r="B32" s="4" t="s">
         <v>2</v>
@@ -2698,7 +2698,7 @@
       <c r="W32" s="3"/>
       <c r="X32" s="3"/>
     </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A33" s="3"/>
       <c r="B33" s="4" t="s">
         <v>0</v>
@@ -2730,10 +2730,10 @@
       <c r="W33" s="3"/>
       <c r="X33" s="3"/>
     </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A34" s="3"/>
       <c r="B34" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C34" s="10" t="s">
         <v>24</v>

</xml_diff>